<commit_message>
modifica logica colonna manuale
</commit_message>
<xml_diff>
--- a/DB/dati_soci.xlsx
+++ b/DB/dati_soci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -61,157 +61,160 @@
     <t>Giuseppe</t>
   </si>
   <si>
+    <t>giuseppe</t>
+  </si>
+  <si>
+    <t>sdsadsa</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>sucuni</t>
+  </si>
+  <si>
     <t>Ci Piace la figa</t>
   </si>
   <si>
-    <t>giuseppe</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>sdsadsa</t>
-  </si>
-  <si>
-    <t>ds</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>sucuni</t>
-  </si>
-  <si>
     <t>Cangemi</t>
   </si>
   <si>
+    <t>cangemi</t>
+  </si>
+  <si>
+    <t>dasdsadsa</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>npizzu</t>
+  </si>
+  <si>
     <t>Tantissimo</t>
   </si>
   <si>
-    <t>cangemi</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>dasdsadsa</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>npizzu</t>
-  </si>
-  <si>
     <t>giuseppecangemi94@gmail.com</t>
   </si>
   <si>
+    <t>giuseppe.cangemi@prova.it</t>
+  </si>
+  <si>
+    <t>dsadadas@sdmsa.it</t>
+  </si>
+  <si>
+    <t>76h@kjjm.it</t>
+  </si>
+  <si>
+    <t>cututtiicugghiunq@sucuni.bisdum</t>
+  </si>
+  <si>
     <t>salvatoremariazuccarello@pornhub.com</t>
   </si>
   <si>
-    <t>giuseppe.cangemi@prova.it</t>
-  </si>
-  <si>
     <t>b@b.it</t>
   </si>
   <si>
-    <t>dsadadas@sdmsa.it</t>
-  </si>
-  <si>
-    <t>76h@kjjm.it</t>
-  </si>
-  <si>
-    <t>cututtiicugghiunq@sucuni.bisdum</t>
+    <t>derryrockfoto.jpg</t>
   </si>
   <si>
     <t>derryrockpubfidelity.png</t>
   </si>
   <si>
-    <t>derryrockfoto.jpg</t>
+    <t>image (31).png</t>
+  </si>
+  <si>
+    <t>image (30).png</t>
+  </si>
+  <si>
+    <t>Immagine 2024-10-31 122037.png</t>
+  </si>
+  <si>
+    <t>image.jpg</t>
   </si>
   <si>
     <t>1000051796.jpg</t>
   </si>
   <si>
-    <t>image (31).png</t>
-  </si>
-  <si>
-    <t>image.jpg</t>
-  </si>
-  <si>
-    <t>image (30).png</t>
-  </si>
-  <si>
-    <t>Immagine 2024-10-31 122037.png</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
     <t>Sì</t>
   </si>
   <si>
+    <t>MOTTA SANT'ANASTASIA</t>
+  </si>
+  <si>
     <t>Milano</t>
   </si>
   <si>
+    <t>dadadas</t>
+  </si>
+  <si>
+    <t>sas</t>
+  </si>
+  <si>
+    <t>carropepe</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>dadadas</t>
-  </si>
-  <si>
-    <t>sas</t>
-  </si>
-  <si>
-    <t>carropepe</t>
-  </si>
-  <si>
-    <t>MOTTA SANT'ANASTASIA</t>
+    <t>e</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
   <si>
     <t>Motta Sant'Anastasia</t>
   </si>
   <si>
+    <t>SAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">misterbianco </t>
+  </si>
+  <si>
     <t>H</t>
   </si>
   <si>
-    <t>SAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">misterbianco </t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>Maschile</t>
   </si>
   <si>
+    <t>Femminile</t>
+  </si>
+  <si>
     <t>Altro</t>
   </si>
   <si>
-    <t>Femminile</t>
+    <t>eee</t>
   </si>
   <si>
     <t>id1234</t>
   </si>
   <si>
+    <t>SAD</t>
+  </si>
+  <si>
+    <t>AHHAHAHAHAHAHA</t>
+  </si>
+  <si>
+    <t>161819273628191</t>
+  </si>
+  <si>
     <t>Jaj</t>
-  </si>
-  <si>
-    <t>SAD</t>
-  </si>
-  <si>
-    <t>AHHAHAHAHAHAHA</t>
-  </si>
-  <si>
-    <t>161819273628191</t>
-  </si>
-  <si>
-    <t>eee</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -625,7 +628,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -643,18 +646,15 @@
         <v>44</v>
       </c>
       <c r="G2">
-        <v>7000</v>
+        <v>3501</v>
       </c>
       <c r="H2" t="s">
         <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -666,170 +666,191 @@
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
         <v>44</v>
       </c>
       <c r="G3">
-        <v>7001</v>
+        <v>7002</v>
       </c>
       <c r="H3" t="s">
         <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2">
+        <v>34681</v>
+      </c>
+      <c r="L3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4">
+        <v>7003</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="2">
+        <v>34315</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="2">
-        <v>34680</v>
-      </c>
-      <c r="L5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" t="s">
-        <v>57</v>
-      </c>
-      <c r="N5" t="s">
-        <v>60</v>
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5">
+        <v>7000</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="2">
-        <v>45573</v>
-      </c>
-      <c r="L6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" t="s">
-        <v>61</v>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6">
+        <v>7001</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7">
-        <v>7001</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K7" s="2">
-        <v>-644653</v>
+        <v>34680</v>
       </c>
       <c r="L7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>44</v>
       </c>
       <c r="G8">
-        <v>7000</v>
+        <v>7001</v>
       </c>
       <c r="H8" t="s">
         <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K8" s="2">
-        <v>-280525</v>
+        <v>-644653</v>
       </c>
       <c r="L8" t="s">
         <v>54</v>
@@ -843,19 +864,19 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
         <v>44</v>
@@ -867,16 +888,16 @@
         <v>44</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K9" s="2">
-        <v>-214781</v>
+        <v>-280525</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="M9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N9" t="s">
         <v>63</v>
@@ -884,118 +905,133 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
         <v>44</v>
       </c>
       <c r="G10">
-        <v>7001</v>
+        <v>7000</v>
       </c>
       <c r="H10" t="s">
         <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K10" s="2">
-        <v>34680</v>
+        <v>-214781</v>
       </c>
       <c r="L10" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="M10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
         <v>44</v>
       </c>
       <c r="G11">
-        <v>666</v>
+        <v>7001</v>
       </c>
       <c r="H11" t="s">
         <v>44</v>
       </c>
-      <c r="I11" t="s">
-        <v>45</v>
-      </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K11" s="2">
-        <v>-5662</v>
+        <v>34680</v>
       </c>
       <c r="L11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M11" t="s">
         <v>58</v>
       </c>
       <c r="N11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
         <v>44</v>
       </c>
       <c r="G12">
-        <v>1201</v>
+        <v>666</v>
       </c>
       <c r="H12" t="s">
         <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="2">
+        <v>-5662</v>
+      </c>
+      <c r="L12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -1007,42 +1043,39 @@
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
       </c>
       <c r="G13">
-        <v>6201</v>
+        <v>1201</v>
       </c>
       <c r="H13" t="s">
         <v>44</v>
-      </c>
-      <c r="I13" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
         <v>44</v>
       </c>
       <c r="G14">
-        <v>3500</v>
+        <v>9999</v>
       </c>
       <c r="H14" t="s">
         <v>44</v>
@@ -1053,33 +1086,48 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
       </c>
       <c r="G15">
-        <v>3501</v>
+        <v>10000</v>
       </c>
       <c r="H15" t="s">
         <v>44</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="2">
+        <v>45573</v>
+      </c>
+      <c r="L15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -1091,31 +1139,48 @@
         <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
         <v>44</v>
       </c>
       <c r="G16">
-        <v>7002</v>
+        <v>6201</v>
       </c>
       <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="J16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="2">
-        <v>34681</v>
-      </c>
-      <c r="L16" t="s">
-        <v>56</v>
-      </c>
-      <c r="M16" t="s">
-        <v>57</v>
-      </c>
-      <c r="N16" t="s">
-        <v>65</v>
+      <c r="I16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17">
+        <v>3500</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifica pdf e logica funzione pdf
</commit_message>
<xml_diff>
--- a/DB/dati_soci.xlsx
+++ b/DB/dati_soci.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -61,16 +61,40 @@
     <t>Giuseppe</t>
   </si>
   <si>
+    <t xml:space="preserve">alessandro </t>
+  </si>
+  <si>
+    <t>serena</t>
+  </si>
+  <si>
     <t>Cangemi</t>
   </si>
   <si>
+    <t>aletta</t>
+  </si>
+  <si>
+    <t>zante</t>
+  </si>
+  <si>
     <t>giuseppecangemi94@gmail.com</t>
   </si>
   <si>
+    <t>abc@prova.it</t>
+  </si>
+  <si>
+    <t>ss@ss.it</t>
+  </si>
+  <si>
+    <t>derryrockpubfidelity.png</t>
+  </si>
+  <si>
+    <t>qrcode_google_form.png</t>
+  </si>
+  <si>
     <t>derryrockfoto.jpg</t>
   </si>
   <si>
-    <t>qrcode_google_form.png</t>
+    <t>image.jpg</t>
   </si>
   <si>
     <t>SI</t>
@@ -85,10 +109,19 @@
     <t>a</t>
   </si>
   <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>e</t>
+    <t>Ss</t>
   </si>
   <si>
     <t>Femminile</t>
@@ -97,10 +130,16 @@
     <t>Maschile</t>
   </si>
   <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
     <t>w</t>
   </si>
   <si>
-    <t>eee</t>
+    <t>Der</t>
   </si>
 </sst>
 </file>
@@ -462,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -514,128 +553,333 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2">
-        <v>34681</v>
+        <v>34679</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2">
         <v>34681</v>
       </c>
       <c r="L3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2">
+        <v>34378</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="2">
+        <v>34649</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="2">
         <v>34681</v>
       </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
         <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="2">
+        <v>34681</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="2">
+        <v>34640</v>
+      </c>
+      <c r="L8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="2">
+        <v>34681</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>